<commit_message>
AJUSTE DIAGRAMA DE CLASE E CRIACAO DICIONARIO DE DADOS
</commit_message>
<xml_diff>
--- a/DOCUMENTOS DA ONG/ASSISTENCIA DIARIA.xlsx
+++ b/DOCUMENTOS DA ONG/ASSISTENCIA DIARIA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\PRE PROJETO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Projeto-ONG\DOCUMENTOS DA ONG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFEA3EA-DC2F-40B4-8E19-A65DB3CF0FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF3DEA5-4D24-439D-8191-D427A3B8B24A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2175" yWindow="-13620" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controle Diario" sheetId="1" r:id="rId1"/>
@@ -1038,14 +1038,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1062,29 +1077,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2805,7 +2805,7 @@
   <dimension ref="A1:W66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9022,13 +9022,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="86"/>
+      <c r="C1" s="75"/>
       <c r="D1" s="63" t="s">
         <v>8</v>
       </c>
@@ -9053,7 +9053,7 @@
       <c r="S1" s="68"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="83"/>
+      <c r="A2" s="72"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
@@ -10000,25 +10000,25 @@
       <c r="S38" s="12"/>
     </row>
     <row r="39" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="79" t="s">
+      <c r="A39" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="80"/>
-      <c r="C39" s="80"/>
-      <c r="D39" s="80"/>
-      <c r="E39" s="80"/>
-      <c r="F39" s="80"/>
-      <c r="G39" s="81"/>
+      <c r="B39" s="77"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="78"/>
     </row>
     <row r="40" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="84" t="s">
+      <c r="A40" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="85"/>
-      <c r="C40" s="85"/>
-      <c r="D40" s="85"/>
-      <c r="E40" s="85"/>
-      <c r="F40" s="85"/>
+      <c r="B40" s="74"/>
+      <c r="C40" s="74"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="74"/>
+      <c r="F40" s="74"/>
       <c r="G40" s="51" t="s">
         <v>29</v>
       </c>
@@ -10261,63 +10261,63 @@
       <c r="G65" s="16"/>
     </row>
     <row r="66" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="71"/>
-      <c r="B66" s="72"/>
-      <c r="C66" s="72"/>
-      <c r="D66" s="72"/>
-      <c r="E66" s="72"/>
-      <c r="F66" s="72"/>
+      <c r="A66" s="84"/>
+      <c r="B66" s="85"/>
+      <c r="C66" s="85"/>
+      <c r="D66" s="85"/>
+      <c r="E66" s="85"/>
+      <c r="F66" s="85"/>
       <c r="G66" s="52"/>
     </row>
     <row r="67" spans="1:19" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="73"/>
-      <c r="B67" s="73"/>
-      <c r="C67" s="73"/>
-      <c r="D67" s="73"/>
-      <c r="E67" s="73"/>
-      <c r="F67" s="73"/>
+      <c r="A67" s="86"/>
+      <c r="B67" s="86"/>
+      <c r="C67" s="86"/>
+      <c r="D67" s="86"/>
+      <c r="E67" s="86"/>
+      <c r="F67" s="86"/>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B68" s="77"/>
-      <c r="C68" s="77"/>
-      <c r="D68" s="77"/>
-      <c r="E68" s="77"/>
-      <c r="F68" s="77"/>
-      <c r="G68" s="77"/>
-      <c r="H68" s="77"/>
-      <c r="I68" s="77"/>
-      <c r="J68" s="77"/>
-      <c r="K68" s="77"/>
-      <c r="L68" s="77"/>
-      <c r="M68" s="77"/>
-      <c r="N68" s="77"/>
-      <c r="O68" s="77"/>
-      <c r="P68" s="77"/>
-      <c r="Q68" s="77"/>
-      <c r="R68" s="77"/>
+      <c r="B68" s="82"/>
+      <c r="C68" s="82"/>
+      <c r="D68" s="82"/>
+      <c r="E68" s="82"/>
+      <c r="F68" s="82"/>
+      <c r="G68" s="82"/>
+      <c r="H68" s="82"/>
+      <c r="I68" s="82"/>
+      <c r="J68" s="82"/>
+      <c r="K68" s="82"/>
+      <c r="L68" s="82"/>
+      <c r="M68" s="82"/>
+      <c r="N68" s="82"/>
+      <c r="O68" s="82"/>
+      <c r="P68" s="82"/>
+      <c r="Q68" s="82"/>
+      <c r="R68" s="82"/>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A69" s="78"/>
-      <c r="B69" s="78"/>
-      <c r="C69" s="78"/>
-      <c r="D69" s="78"/>
-      <c r="E69" s="78"/>
-      <c r="F69" s="78"/>
-      <c r="G69" s="78"/>
-      <c r="H69" s="78"/>
-      <c r="I69" s="78"/>
-      <c r="J69" s="78"/>
-      <c r="K69" s="78"/>
-      <c r="L69" s="78"/>
-      <c r="M69" s="78"/>
-      <c r="N69" s="78"/>
-      <c r="O69" s="78"/>
-      <c r="P69" s="78"/>
-      <c r="Q69" s="78"/>
-      <c r="R69" s="78"/>
+      <c r="A69" s="83"/>
+      <c r="B69" s="83"/>
+      <c r="C69" s="83"/>
+      <c r="D69" s="83"/>
+      <c r="E69" s="83"/>
+      <c r="F69" s="83"/>
+      <c r="G69" s="83"/>
+      <c r="H69" s="83"/>
+      <c r="I69" s="83"/>
+      <c r="J69" s="83"/>
+      <c r="K69" s="83"/>
+      <c r="L69" s="83"/>
+      <c r="M69" s="83"/>
+      <c r="N69" s="83"/>
+      <c r="O69" s="83"/>
+      <c r="P69" s="83"/>
+      <c r="Q69" s="83"/>
+      <c r="R69" s="83"/>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="10"/>
@@ -10340,43 +10340,47 @@
       <c r="R70" s="12"/>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A71" s="74" t="s">
+      <c r="A71" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="B71" s="74"/>
-      <c r="C71" s="74"/>
-      <c r="D71" s="76"/>
-      <c r="E71" s="76"/>
-      <c r="F71" s="76"/>
-      <c r="G71" s="76"/>
-      <c r="H71" s="76"/>
-      <c r="I71" s="75" t="s">
+      <c r="B71" s="79"/>
+      <c r="C71" s="79"/>
+      <c r="D71" s="81"/>
+      <c r="E71" s="81"/>
+      <c r="F71" s="81"/>
+      <c r="G71" s="81"/>
+      <c r="H71" s="81"/>
+      <c r="I71" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="J71" s="75"/>
-      <c r="K71" s="75"/>
-      <c r="L71" s="75"/>
-      <c r="M71" s="75"/>
-      <c r="N71" s="75"/>
-      <c r="O71" s="76"/>
-      <c r="P71" s="76"/>
-      <c r="Q71" s="76"/>
-      <c r="R71" s="76"/>
-      <c r="S71" s="76"/>
+      <c r="J71" s="80"/>
+      <c r="K71" s="80"/>
+      <c r="L71" s="80"/>
+      <c r="M71" s="80"/>
+      <c r="N71" s="80"/>
+      <c r="O71" s="81"/>
+      <c r="P71" s="81"/>
+      <c r="Q71" s="81"/>
+      <c r="R71" s="81"/>
+      <c r="S71" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="H1:N1"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A56:F56"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="O1:S1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A64:F64"/>
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="A67:F67"/>
+    <mergeCell ref="A59:F59"/>
+    <mergeCell ref="A60:F60"/>
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="I71:N71"/>
+    <mergeCell ref="O71:S71"/>
+    <mergeCell ref="D71:H71"/>
+    <mergeCell ref="B68:R68"/>
+    <mergeCell ref="A69:R69"/>
     <mergeCell ref="A58:F58"/>
     <mergeCell ref="A39:G39"/>
     <mergeCell ref="A50:F50"/>
@@ -10391,21 +10395,17 @@
     <mergeCell ref="A49:F49"/>
     <mergeCell ref="A42:F42"/>
     <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="I71:N71"/>
-    <mergeCell ref="O71:S71"/>
-    <mergeCell ref="D71:H71"/>
-    <mergeCell ref="B68:R68"/>
-    <mergeCell ref="A69:R69"/>
-    <mergeCell ref="A64:F64"/>
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="A66:F66"/>
-    <mergeCell ref="A67:F67"/>
-    <mergeCell ref="A59:F59"/>
-    <mergeCell ref="A60:F60"/>
-    <mergeCell ref="A61:F61"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="H1:N1"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A56:F56"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="O1:S1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:G1"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.74803149606299213" bottom="0.27559055118110237" header="7.874015748031496E-2" footer="0.11811023622047245"/>

</xml_diff>